<commit_message>
new maps with pie charts
Pie charts
- show when there are at least 3 translations
- show every language that is in the legend, otherwise 'other language'
- Czechia gray
- transparency 0.5
</commit_message>
<xml_diff>
--- a/geotagged/countries_info_new.xlsx
+++ b/geotagged/countries_info_new.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlottepanuskova/Nextcloud/translation-mapping/geotagged/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3CF83E-9DAE-5E4A-872D-92B1144128BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E053F05-78BA-5844-AD07-A61BB094C5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$V$250</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -7550,10 +7553,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:V250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="N207" sqref="N207"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M270" sqref="M270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7632,7 +7636,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -7685,7 +7689,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -7750,7 +7754,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
@@ -7809,7 +7813,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>59</v>
       </c>
@@ -7871,7 +7875,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>71</v>
       </c>
@@ -7933,7 +7937,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>83</v>
       </c>
@@ -7998,7 +8002,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>93</v>
       </c>
@@ -8060,7 +8064,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>104</v>
       </c>
@@ -8122,7 +8126,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>113</v>
       </c>
@@ -8184,7 +8188,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>123</v>
       </c>
@@ -8246,7 +8250,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>135</v>
       </c>
@@ -8302,7 +8306,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>144</v>
       </c>
@@ -8364,7 +8368,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>154</v>
       </c>
@@ -8420,7 +8424,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>164</v>
       </c>
@@ -8482,7 +8486,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>177</v>
       </c>
@@ -8538,7 +8542,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>188</v>
       </c>
@@ -8594,7 +8598,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>197</v>
       </c>
@@ -8656,7 +8660,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>205</v>
       </c>
@@ -8718,7 +8722,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>216</v>
       </c>
@@ -8774,7 +8778,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>225</v>
       </c>
@@ -8830,7 +8834,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>237</v>
       </c>
@@ -8892,7 +8896,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>247</v>
       </c>
@@ -8948,7 +8952,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>256</v>
       </c>
@@ -9001,7 +9005,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>266</v>
       </c>
@@ -9057,7 +9061,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>274</v>
       </c>
@@ -9113,7 +9117,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>282</v>
       </c>
@@ -9175,7 +9179,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>296</v>
       </c>
@@ -9237,7 +9241,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>311</v>
       </c>
@@ -9299,7 +9303,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>323</v>
       </c>
@@ -9352,7 +9356,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>335</v>
       </c>
@@ -9414,7 +9418,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>346</v>
       </c>
@@ -9476,7 +9480,7 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>356</v>
       </c>
@@ -9538,7 +9542,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>370</v>
       </c>
@@ -9597,7 +9601,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>380</v>
       </c>
@@ -9659,7 +9663,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>394</v>
       </c>
@@ -9721,7 +9725,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>405</v>
       </c>
@@ -9783,7 +9787,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>417</v>
       </c>
@@ -9845,7 +9849,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>426</v>
       </c>
@@ -9907,7 +9911,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>435</v>
       </c>
@@ -9969,7 +9973,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>446</v>
       </c>
@@ -10031,7 +10035,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>455</v>
       </c>
@@ -10090,7 +10094,7 @@
         <v>2374</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>464</v>
       </c>
@@ -10146,7 +10150,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>474</v>
       </c>
@@ -10205,7 +10209,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>482</v>
       </c>
@@ -10267,7 +10271,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>491</v>
       </c>
@@ -10317,7 +10321,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>499</v>
       </c>
@@ -10373,7 +10377,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>508</v>
       </c>
@@ -10423,7 +10427,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>516</v>
       </c>
@@ -10473,7 +10477,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>524</v>
       </c>
@@ -10532,7 +10536,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>535</v>
       </c>
@@ -10591,7 +10595,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>542</v>
       </c>
@@ -10647,7 +10651,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>552</v>
       </c>
@@ -10703,7 +10707,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>562</v>
       </c>
@@ -10753,7 +10757,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>571</v>
       </c>
@@ -10809,7 +10813,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>582</v>
       </c>
@@ -10862,7 +10866,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>591</v>
       </c>
@@ -10921,7 +10925,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>603</v>
       </c>
@@ -10974,7 +10978,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>612</v>
       </c>
@@ -11030,7 +11034,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>620</v>
       </c>
@@ -11080,7 +11084,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>628</v>
       </c>
@@ -11133,7 +11137,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>636</v>
       </c>
@@ -11186,7 +11190,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>644</v>
       </c>
@@ -11242,7 +11246,7 @@
         <v>2081918</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>651</v>
       </c>
@@ -11304,7 +11308,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>662</v>
       </c>
@@ -11354,7 +11358,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>670</v>
       </c>
@@ -11410,7 +11414,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>680</v>
       </c>
@@ -11466,7 +11470,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>688</v>
       </c>
@@ -11522,7 +11526,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>697</v>
       </c>
@@ -11581,7 +11585,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>708</v>
       </c>
@@ -11637,7 +11641,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>717</v>
       </c>
@@ -11699,7 +11703,7 @@
         <v>2375</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>726</v>
       </c>
@@ -11752,7 +11756,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>733</v>
       </c>
@@ -11802,7 +11806,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>741</v>
       </c>
@@ -11855,7 +11859,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>749</v>
       </c>
@@ -11905,7 +11909,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>757</v>
       </c>
@@ -11955,7 +11959,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>766</v>
       </c>
@@ -12005,7 +12009,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>774</v>
       </c>
@@ -12129,7 +12133,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>793</v>
       </c>
@@ -12179,7 +12183,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>801</v>
       </c>
@@ -12232,7 +12236,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>810</v>
       </c>
@@ -12285,7 +12289,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>819</v>
       </c>
@@ -12344,7 +12348,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>825</v>
       </c>
@@ -12406,7 +12410,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>836</v>
       </c>
@@ -12465,7 +12469,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>843</v>
       </c>
@@ -12518,7 +12522,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>851</v>
       </c>
@@ -12574,7 +12578,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>861</v>
       </c>
@@ -12627,7 +12631,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>870</v>
       </c>
@@ -12680,7 +12684,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>878</v>
       </c>
@@ -12739,7 +12743,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>888</v>
       </c>
@@ -12795,7 +12799,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>898</v>
       </c>
@@ -12857,7 +12861,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>910</v>
       </c>
@@ -12913,7 +12917,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>920</v>
       </c>
@@ -12963,7 +12967,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>928</v>
       </c>
@@ -13010,7 +13014,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>933</v>
       </c>
@@ -13069,7 +13073,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>940</v>
       </c>
@@ -13119,7 +13123,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>947</v>
       </c>
@@ -13169,7 +13173,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>955</v>
       </c>
@@ -13225,7 +13229,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>963</v>
       </c>
@@ -13287,7 +13291,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>973</v>
       </c>
@@ -13343,7 +13347,7 @@
         <v>2376</v>
       </c>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>983</v>
       </c>
@@ -13402,7 +13406,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>991</v>
       </c>
@@ -13461,7 +13465,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>999</v>
       </c>
@@ -13520,7 +13524,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>1007</v>
       </c>
@@ -13576,7 +13580,7 @@
         <v>2078138</v>
       </c>
     </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>1014</v>
       </c>
@@ -13638,7 +13642,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>1027</v>
       </c>
@@ -13694,7 +13698,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>1038</v>
       </c>
@@ -13756,7 +13760,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>1050</v>
       </c>
@@ -13818,7 +13822,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>1059</v>
       </c>
@@ -13877,7 +13881,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>1069</v>
       </c>
@@ -13936,7 +13940,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="112" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>1079</v>
       </c>
@@ -13995,7 +13999,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="113" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>1088</v>
       </c>
@@ -14057,7 +14061,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="114" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>1098</v>
       </c>
@@ -14119,7 +14123,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="115" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>1106</v>
       </c>
@@ -14175,7 +14179,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="116" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>1115</v>
       </c>
@@ -14234,7 +14238,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="117" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>1125</v>
       </c>
@@ -14293,7 +14297,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="118" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>1138</v>
       </c>
@@ -14352,7 +14356,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="119" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>1147</v>
       </c>
@@ -14411,7 +14415,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="120" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>1158</v>
       </c>
@@ -14470,7 +14474,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="121" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>1169</v>
       </c>
@@ -14532,7 +14536,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="122" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>1179</v>
       </c>
@@ -14594,7 +14598,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="123" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>1190</v>
       </c>
@@ -14653,7 +14657,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="124" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>1200</v>
       </c>
@@ -14715,7 +14719,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="125" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>1209</v>
       </c>
@@ -14777,7 +14781,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="126" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>1219</v>
       </c>
@@ -14839,7 +14843,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="127" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>1229</v>
       </c>
@@ -14895,7 +14899,7 @@
         <v>2377</v>
       </c>
     </row>
-    <row r="128" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>1238</v>
       </c>
@@ -14957,7 +14961,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="129" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>1250</v>
       </c>
@@ -15019,7 +15023,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="130" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>1260</v>
       </c>
@@ -15078,7 +15082,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="131" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>1268</v>
       </c>
@@ -15137,7 +15141,7 @@
         <v>1276</v>
       </c>
     </row>
-    <row r="132" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>1277</v>
       </c>
@@ -15193,7 +15197,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="133" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>1285</v>
       </c>
@@ -15252,7 +15256,7 @@
         <v>2378</v>
       </c>
     </row>
-    <row r="134" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>1290</v>
       </c>
@@ -15302,7 +15306,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="135" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>1296</v>
       </c>
@@ -15358,7 +15362,7 @@
         <v>2379</v>
       </c>
     </row>
-    <row r="136" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>1305</v>
       </c>
@@ -15414,7 +15418,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="137" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>1315</v>
       </c>
@@ -15470,7 +15474,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="138" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>1324</v>
       </c>
@@ -15526,7 +15530,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="139" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>1333</v>
       </c>
@@ -15582,7 +15586,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="140" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>1341</v>
       </c>
@@ -15638,7 +15642,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="141" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>1349</v>
       </c>
@@ -15700,7 +15704,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="142" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>1357</v>
       </c>
@@ -15756,7 +15760,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="143" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>1364</v>
       </c>
@@ -15818,7 +15822,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="144" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>1374</v>
       </c>
@@ -15874,7 +15878,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="145" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>1384</v>
       </c>
@@ -15930,7 +15934,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="146" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>1390</v>
       </c>
@@ -15992,7 +15996,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="147" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>1397</v>
       </c>
@@ -16051,7 +16055,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="148" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>1406</v>
       </c>
@@ -16107,7 +16111,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="149" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>1414</v>
       </c>
@@ -16163,7 +16167,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="150" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>1422</v>
       </c>
@@ -16222,7 +16226,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="151" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>1430</v>
       </c>
@@ -16284,7 +16288,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="152" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>1438</v>
       </c>
@@ -16343,7 +16347,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="153" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>1447</v>
       </c>
@@ -16399,7 +16403,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="154" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>1454</v>
       </c>
@@ -16458,7 +16462,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="155" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>1462</v>
       </c>
@@ -16520,7 +16524,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="156" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>1469</v>
       </c>
@@ -16576,7 +16580,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="157" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>1478</v>
       </c>
@@ -16635,7 +16639,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="158" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>1484</v>
       </c>
@@ -16697,7 +16701,7 @@
         <v>1494</v>
       </c>
     </row>
-    <row r="159" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>1495</v>
       </c>
@@ -16759,7 +16763,7 @@
         <v>1504</v>
       </c>
     </row>
-    <row r="160" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>1505</v>
       </c>
@@ -16821,7 +16825,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="161" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>1516</v>
       </c>
@@ -16883,7 +16887,7 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="162" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>1526</v>
       </c>
@@ -16942,7 +16946,7 @@
         <v>1537</v>
       </c>
     </row>
-    <row r="163" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>1538</v>
       </c>
@@ -17004,7 +17008,7 @@
         <v>1548</v>
       </c>
     </row>
-    <row r="164" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>1549</v>
       </c>
@@ -17066,7 +17070,7 @@
         <v>1559</v>
       </c>
     </row>
-    <row r="165" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>1560</v>
       </c>
@@ -17128,7 +17132,7 @@
         <v>1569</v>
       </c>
     </row>
-    <row r="166" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>1570</v>
       </c>
@@ -17187,7 +17191,7 @@
         <v>1579</v>
       </c>
     </row>
-    <row r="167" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>1580</v>
       </c>
@@ -17249,7 +17253,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="168" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>1589</v>
       </c>
@@ -17311,7 +17315,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="169" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>1597</v>
       </c>
@@ -17370,7 +17374,7 @@
         <v>1609</v>
       </c>
     </row>
-    <row r="170" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>1610</v>
       </c>
@@ -17432,7 +17436,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="171" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>1620</v>
       </c>
@@ -17494,7 +17498,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="172" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>1631</v>
       </c>
@@ -17550,7 +17554,7 @@
         <v>2382</v>
       </c>
     </row>
-    <row r="173" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>1638</v>
       </c>
@@ -17612,7 +17616,7 @@
         <v>2383</v>
       </c>
     </row>
-    <row r="174" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>1649</v>
       </c>
@@ -17674,7 +17678,7 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="175" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>1661</v>
       </c>
@@ -17736,7 +17740,7 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="176" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>1669</v>
       </c>
@@ -17798,7 +17802,7 @@
         <v>1679</v>
       </c>
     </row>
-    <row r="177" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>1680</v>
       </c>
@@ -17860,7 +17864,7 @@
         <v>2384</v>
       </c>
     </row>
-    <row r="178" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>1688</v>
       </c>
@@ -17922,7 +17926,7 @@
         <v>2385</v>
       </c>
     </row>
-    <row r="179" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>1697</v>
       </c>
@@ -17978,7 +17982,7 @@
         <v>1707</v>
       </c>
     </row>
-    <row r="180" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>1708</v>
       </c>
@@ -18040,7 +18044,7 @@
         <v>1718</v>
       </c>
     </row>
-    <row r="181" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>1719</v>
       </c>
@@ -18102,7 +18106,7 @@
         <v>1729</v>
       </c>
     </row>
-    <row r="182" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>1730</v>
       </c>
@@ -18164,7 +18168,7 @@
         <v>1741</v>
       </c>
     </row>
-    <row r="183" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>1742</v>
       </c>
@@ -18223,7 +18227,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="184" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>1751</v>
       </c>
@@ -18285,7 +18289,7 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="185" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>1761</v>
       </c>
@@ -18347,7 +18351,7 @@
         <v>1770</v>
       </c>
     </row>
-    <row r="186" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>1771</v>
       </c>
@@ -18409,7 +18413,7 @@
         <v>1780</v>
       </c>
     </row>
-    <row r="187" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>1781</v>
       </c>
@@ -18459,7 +18463,7 @@
         <v>1547376</v>
       </c>
     </row>
-    <row r="188" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>1787</v>
       </c>
@@ -18521,7 +18525,7 @@
         <v>1780</v>
       </c>
     </row>
-    <row r="189" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>1796</v>
       </c>
@@ -18580,7 +18584,7 @@
         <v>1805</v>
       </c>
     </row>
-    <row r="190" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>1806</v>
       </c>
@@ -18642,7 +18646,7 @@
         <v>1816</v>
       </c>
     </row>
-    <row r="191" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>1817</v>
       </c>
@@ -18695,7 +18699,7 @@
         <v>2386</v>
       </c>
     </row>
-    <row r="192" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>1824</v>
       </c>
@@ -18757,7 +18761,7 @@
         <v>1832</v>
       </c>
     </row>
-    <row r="193" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>1833</v>
       </c>
@@ -18810,7 +18814,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="194" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>1839</v>
       </c>
@@ -18863,7 +18867,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="195" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>1848</v>
       </c>
@@ -18913,7 +18917,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="196" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>1858</v>
       </c>
@@ -18975,7 +18979,7 @@
         <v>1866</v>
       </c>
     </row>
-    <row r="197" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>1867</v>
       </c>
@@ -19037,7 +19041,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="198" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>1877</v>
       </c>
@@ -19093,7 +19097,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="199" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>1887</v>
       </c>
@@ -19146,7 +19150,7 @@
         <v>1893</v>
       </c>
     </row>
-    <row r="200" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>1894</v>
       </c>
@@ -19196,7 +19200,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="201" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>1901</v>
       </c>
@@ -19240,7 +19244,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="202" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>1906</v>
       </c>
@@ -19302,7 +19306,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="203" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>1916</v>
       </c>
@@ -19361,7 +19365,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="204" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>1922</v>
       </c>
@@ -19423,7 +19427,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="205" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>1932</v>
       </c>
@@ -19482,7 +19486,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="206" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>1941</v>
       </c>
@@ -19544,7 +19548,7 @@
         <v>1953</v>
       </c>
     </row>
-    <row r="207" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>1954</v>
       </c>
@@ -19600,7 +19604,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="208" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>1965</v>
       </c>
@@ -19662,7 +19666,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="209" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>1977</v>
       </c>
@@ -19721,7 +19725,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="210" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>1986</v>
       </c>
@@ -19783,7 +19787,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="211" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>1995</v>
       </c>
@@ -19845,7 +19849,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="212" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>2005</v>
       </c>
@@ -19907,7 +19911,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="213" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>2015</v>
       </c>
@@ -19960,7 +19964,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="214" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>2024</v>
       </c>
@@ -20022,7 +20026,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="215" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>2035</v>
       </c>
@@ -20084,7 +20088,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="216" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>2046</v>
       </c>
@@ -20146,7 +20150,7 @@
         <v>2056</v>
       </c>
     </row>
-    <row r="217" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>2057</v>
       </c>
@@ -20202,7 +20206,7 @@
         <v>2066</v>
       </c>
     </row>
-    <row r="218" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>2067</v>
       </c>
@@ -20258,7 +20262,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="219" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>2076</v>
       </c>
@@ -20317,7 +20321,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="220" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>2086</v>
       </c>
@@ -20379,7 +20383,7 @@
         <v>2095</v>
       </c>
     </row>
-    <row r="221" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>2096</v>
       </c>
@@ -20441,7 +20445,7 @@
         <v>2387</v>
       </c>
     </row>
-    <row r="222" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>2105</v>
       </c>
@@ -20494,7 +20498,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="223" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>2114</v>
       </c>
@@ -20556,7 +20560,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="224" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>2126</v>
       </c>
@@ -20618,7 +20622,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="225" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>2137</v>
       </c>
@@ -20668,7 +20672,7 @@
         <v>2144</v>
       </c>
     </row>
-    <row r="226" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>2145</v>
       </c>
@@ -20730,7 +20734,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="227" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>2151</v>
       </c>
@@ -20792,7 +20796,7 @@
         <v>2373</v>
       </c>
     </row>
-    <row r="228" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>2160</v>
       </c>
@@ -20851,7 +20855,7 @@
         <v>2167</v>
       </c>
     </row>
-    <row r="229" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>2168</v>
       </c>
@@ -20913,7 +20917,7 @@
         <v>2167</v>
       </c>
     </row>
-    <row r="230" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>2178</v>
       </c>
@@ -20975,7 +20979,7 @@
         <v>2187</v>
       </c>
     </row>
-    <row r="231" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>2188</v>
       </c>
@@ -21031,7 +21035,7 @@
         <v>2187</v>
       </c>
     </row>
-    <row r="232" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>2197</v>
       </c>
@@ -21087,7 +21091,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="233" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>2204</v>
       </c>
@@ -21149,7 +21153,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="234" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>2216</v>
       </c>
@@ -21211,7 +21215,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="235" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>2227</v>
       </c>
@@ -21273,7 +21277,7 @@
         <v>2237</v>
       </c>
     </row>
-    <row r="236" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>2238</v>
       </c>
@@ -21323,7 +21327,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="237" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>2243</v>
       </c>
@@ -21382,7 +21386,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="238" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>2252</v>
       </c>
@@ -21435,7 +21439,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="239" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>2260</v>
       </c>
@@ -21497,7 +21501,7 @@
         <v>2271</v>
       </c>
     </row>
-    <row r="240" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>2272</v>
       </c>
@@ -21550,7 +21554,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="241" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>2279</v>
       </c>
@@ -21612,7 +21616,7 @@
         <v>2290</v>
       </c>
     </row>
-    <row r="242" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>2291</v>
       </c>
@@ -21674,7 +21678,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="243" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>2301</v>
       </c>
@@ -21736,7 +21740,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="244" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>2311</v>
       </c>
@@ -21798,7 +21802,7 @@
         <v>2322</v>
       </c>
     </row>
-    <row r="245" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>2323</v>
       </c>
@@ -21857,7 +21861,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="246" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>2331</v>
       </c>
@@ -21919,7 +21923,7 @@
         <v>2340</v>
       </c>
     </row>
-    <row r="247" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
         <v>2341</v>
       </c>
@@ -21972,7 +21976,7 @@
         <v>2340</v>
       </c>
     </row>
-    <row r="248" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>2348</v>
       </c>
@@ -22031,7 +22035,7 @@
         <v>2340</v>
       </c>
     </row>
-    <row r="249" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
         <v>2356</v>
       </c>
@@ -22084,7 +22088,7 @@
         <v>2340</v>
       </c>
     </row>
-    <row r="250" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
         <v>2363</v>
       </c>
@@ -22147,6 +22151,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:V250" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Lesotho"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>